<commit_message>
Added punctuation to keeling CLR
</commit_message>
<xml_diff>
--- a/keeling/CLR/CLR_keeling.xlsx
+++ b/keeling/CLR/CLR_keeling.xlsx
@@ -2143,14 +2143,14 @@
     <t>Keeling, Ralph F; Keeling, Charles D (2017): Scripps CO2 Program Data. UC San Diego Library Digital Collections.</t>
   </si>
   <si>
+    <t xml:space="preserve">
+The Scripps CO2 Program website at &lt;a href="http://scrippsco2.ucsd.edu"&gt;http://scrippsco2.ucsd.edu&lt;/a&gt; provides access to openly available atmospheric and seawater CO2 concentration data from various sources. Redundant copies of the atmospheric CO2 data from 13 sampling stations are being deposited here, through the UC San Diego Library, to provide enhanced discovery, long-term accessibility, and preservation.</t>
+  </si>
+  <si>
     <t>The Scripps CO2 Program was initiated in 1956 by Charles David Keeling and operated under his direction until his passing in 2005. It is currently being continued by Ralph F. Keeling, who also runs a parallel program at Scripps Institution of Oceanography to measure changes in atmospheric O2 and Ar abundances (&lt;a href="http://scrippso2.ucsd.edu"&gt;Scripps O2 Program&lt;/a&gt;).
 Current results, including data sets and graphics, are available at &lt;a href="http://scrippsco2.ucsd.edu"&gt; http://scrippsco2.ucsd.edu&lt;/a&gt; from the ongoing program to measure CO2 and chemical species. 
-For daily updates of the CO2 Concentration at Mauna Loa Obervatory, Hawaii, see &lt;a href="https://scripps.ucsd.edu/programs/keelingcurve/"&gt;keelingcurve.ucsd.edu&lt;/a&gt; .
+For daily updates of the CO2 Concentration at Mauna Loa Obervatory, Hawaii, see &lt;a href="https://scripps.ucsd.edu/programs/keelingcurve/"&gt;keelingcurve.ucsd.edu&lt;/a&gt;.
 Measurements of atmospheric CO2 concentration in our program began in 1957 at La Jolla, California and at the South Pole, and in 1958 at Mauna Loa Observatory. These measurements were gradually extended during the 1960's and 1970's to comprise sampling at an array of stations from the Arctic to Antarctica.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-The Scripps CO2 Program website at &lt;a href="http://scrippsco2.ucsd.edu"&gt;http://scrippsco2.ucsd.edu&lt;/a&gt; provides access to openly available atmospheric and seawater CO2 concentration data from various sources. Redundant copies of the atmospheric CO2 data from 13 sampling stations are being deposited here, through the UC San Diego Library, to provide enhanced discovery, long-term accessibility, and preservation.</t>
   </si>
 </sst>
 </file>
@@ -3218,8 +3218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3356,10 +3356,10 @@
         <v>648</v>
       </c>
       <c r="O2" s="23" t="s">
+        <v>650</v>
+      </c>
+      <c r="P2" s="23" t="s">
         <v>649</v>
-      </c>
-      <c r="P2" s="23" t="s">
-        <v>650</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>639</v>

</xml_diff>